<commit_message>
Second stab fix bullet point cebad50be0dc2bd4a84c6c5b3eee6d3547470c3b
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/StructureDefinition-fr-requestgroup-for-prescription.xlsx
+++ b/FinalisationMappingPosologie/ig/StructureDefinition-fr-requestgroup-for-prescription.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>RequestGroup for prescription</t>
+    <t>FrRequestGroupForPrescrption</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-14T13:17:43+00:00</t>
+    <t>2025-04-14T13:53:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>